<commit_message>
Added the transformation script
</commit_message>
<xml_diff>
--- a/input_data/team_brain_n_bytes_data.xlsx
+++ b/input_data/team_brain_n_bytes_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SyedAtyabHussain\Documents\team_brain_and_bytes_work_area\monthly_performance_reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SyedAtyabHussain\Documents\work_area\PerformanceReportGenerator\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{963D49B5-C4D0-472E-BDAF-7B8EBAA87910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE7693C-15C3-44C3-938E-5AE2AC2B2E6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="6" activeTab="6" xr2:uid="{63149AD4-535C-4F32-A263-C64852C93E16}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{63149AD4-535C-4F32-A263-C64852C93E16}"/>
   </bookViews>
   <sheets>
     <sheet name="April 2025" sheetId="1" r:id="rId1"/>
@@ -895,9 +895,6 @@
   </si>
   <si>
     <t>Consistently punctual and meets all deadlines.</t>
-  </si>
-  <si>
-    <t>Srpint No.</t>
   </si>
   <si>
     <t>Sprint URL</t>
@@ -1355,6 +1352,9 @@
   <si>
     <t>97.96%%</t>
   </si>
+  <si>
+    <t>Sprint No.</t>
+  </si>
 </sst>
 </file>
 
@@ -1363,7 +1363,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2514,30 +2514,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{724D366B-9E52-4CC7-9A86-6B34AE509C5C}">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" sqref="A1:A1048576"/>
+      <selection pane="topRight" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="75.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="68.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="72.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="63.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="75.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="68.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="63.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="80" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="73.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="61.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="73.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="61.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="72" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="60.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="61.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="46.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="36.140625" style="6" customWidth="1"/>
-    <col min="15" max="15" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="60.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="61.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="36.109375" style="6" customWidth="1"/>
+    <col min="15" max="15" width="20.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18">
+    <row r="1" spans="1:14" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2581,7 +2581,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
@@ -2625,7 +2625,7 @@
         <v>33.522727272727273</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>10.227272727272728</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
@@ -2713,7 +2713,7 @@
         <v>9.0909090909090917</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>53</v>
       </c>
@@ -2757,7 +2757,7 @@
         <v>13.636363636363635</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>66</v>
       </c>
@@ -2801,7 +2801,7 @@
         <v>20.454545454545457</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>79</v>
       </c>
@@ -2845,7 +2845,7 @@
         <v>6.8181818181818175</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>92</v>
       </c>
@@ -2889,7 +2889,7 @@
         <v>30.681818181818183</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>105</v>
       </c>
@@ -2933,7 +2933,7 @@
         <v>19.318181818181817</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>118</v>
       </c>
@@ -2977,7 +2977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>131</v>
       </c>
@@ -3021,7 +3021,7 @@
         <v>10.795454545454545</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>144</v>
       </c>
@@ -3065,7 +3065,7 @@
         <v>17.045454545454543</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>157</v>
       </c>
@@ -3109,7 +3109,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="15">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>170</v>
       </c>
@@ -3153,7 +3153,7 @@
         <v>21.59090909090909</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>182</v>
       </c>
@@ -3197,7 +3197,7 @@
         <v>44.31818181818182</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>195</v>
       </c>
@@ -3241,7 +3241,7 @@
         <v>15.909090909090908</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>207</v>
       </c>
@@ -3285,7 +3285,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>219</v>
       </c>
@@ -3329,7 +3329,7 @@
         <v>13.636363636363635</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="15">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>229</v>
       </c>
@@ -3373,7 +3373,7 @@
         <v>10.227272727272728</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="15">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>241</v>
       </c>
@@ -3417,7 +3417,7 @@
         <v>6.8181818181818175</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="15">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>254</v>
       </c>
@@ -3461,7 +3461,7 @@
         <v>15.909090909090908</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>267</v>
       </c>
@@ -3505,7 +3505,7 @@
         <v>17.045454545454543</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>270</v>
       </c>
@@ -3549,7 +3549,7 @@
         <v>19.318181818181817</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="15">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>271</v>
       </c>
@@ -3593,80 +3593,80 @@
         <v>22.727272727272727</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="C27" s="3" t="s">
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="28" spans="1:14">
-      <c r="A28" s="3" t="s">
+      <c r="B28" t="s">
         <v>287</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>288</v>
       </c>
-      <c r="C28" t="s">
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="29" spans="1:14">
-      <c r="A29" s="3" t="s">
+      <c r="B29" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="C29" t="s">
         <v>291</v>
       </c>
-      <c r="C29" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14">
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="1:14" ht="15">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="C32" t="s">
         <v>294</v>
       </c>
-      <c r="C32" t="s">
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="15">
-      <c r="A33" s="3" t="s">
+      <c r="B33" s="27" t="s">
         <v>296</v>
-      </c>
-      <c r="B33" s="27" t="s">
-        <v>297</v>
       </c>
       <c r="C33" s="27"/>
       <c r="D33" s="27"/>
@@ -3687,30 +3687,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0339E0F6-DA40-4AC3-BE85-360C2D887690}">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B20" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="75.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="68.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="72.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="63.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="75.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="68.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="63.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="80" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="73.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="61.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="73.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="61.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="72" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="60.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="61.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="46.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="36.140625" style="6" customWidth="1"/>
-    <col min="15" max="15" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="60.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="61.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="36.109375" style="6" customWidth="1"/>
+    <col min="15" max="15" width="20.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18">
+    <row r="1" spans="1:14" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3754,7 +3754,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
@@ -3798,7 +3798,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
@@ -3842,7 +3842,7 @@
         <v>72.02</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
@@ -3886,7 +3886,7 @@
         <v>89.29</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>53</v>
       </c>
@@ -3930,7 +3930,7 @@
         <v>69.05</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>66</v>
       </c>
@@ -3974,7 +3974,7 @@
         <v>72.62</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>79</v>
       </c>
@@ -4018,7 +4018,7 @@
         <v>70.239999999999995</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>92</v>
       </c>
@@ -4062,7 +4062,7 @@
         <v>61.9</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>105</v>
       </c>
@@ -4106,7 +4106,7 @@
         <v>65.48</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>118</v>
       </c>
@@ -4150,7 +4150,7 @@
         <v>54.76</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>131</v>
       </c>
@@ -4191,10 +4191,10 @@
         <v>143</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>144</v>
       </c>
@@ -4238,7 +4238,7 @@
         <v>90.48</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>157</v>
       </c>
@@ -4282,7 +4282,7 @@
         <v>57.14</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>170</v>
       </c>
@@ -4326,7 +4326,7 @@
         <v>95.24</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>182</v>
       </c>
@@ -4370,7 +4370,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>195</v>
       </c>
@@ -4414,7 +4414,7 @@
         <v>44.05</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>207</v>
       </c>
@@ -4458,7 +4458,7 @@
         <v>86.31</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>219</v>
       </c>
@@ -4502,7 +4502,7 @@
         <v>43.45</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>229</v>
       </c>
@@ -4546,7 +4546,7 @@
         <v>26.79</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>241</v>
       </c>
@@ -4590,7 +4590,7 @@
         <v>61.9</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>254</v>
       </c>
@@ -4634,7 +4634,7 @@
         <v>87.5</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>267</v>
       </c>
@@ -4678,7 +4678,7 @@
         <v>65.48</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>270</v>
       </c>
@@ -4722,7 +4722,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>271</v>
       </c>
@@ -4766,83 +4766,83 @@
         <v>48.21</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="14.45">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="1:14" ht="14.45">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>286</v>
-      </c>
       <c r="D27" s="3" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="28" spans="1:14">
-      <c r="A28" s="3" t="s">
+      <c r="B28" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="C28" t="s">
         <v>301</v>
       </c>
-      <c r="C28" t="s">
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="29" spans="1:14">
-      <c r="A29" s="3" t="s">
+      <c r="B29" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="C29" t="s">
         <v>304</v>
       </c>
-      <c r="C29" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" ht="14.45">
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="1:14" ht="14.45" customHeight="1">
+    <row r="32" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="C32" t="s">
         <v>294</v>
       </c>
-      <c r="C32" t="s">
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="8" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="8" t="s">
+      <c r="B33" s="27" t="s">
         <v>296</v>
-      </c>
-      <c r="B33" s="27" t="s">
-        <v>297</v>
       </c>
       <c r="C33" s="27"/>
       <c r="D33" s="27"/>
@@ -4865,29 +4865,29 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B20" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B29" sqref="B29"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="75.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="68.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="72.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="63.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="75.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="68.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="63.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="80" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="73.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="61.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="73.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="61.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="72" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="60.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="61.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="46.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="36.140625" style="6" customWidth="1"/>
-    <col min="15" max="15" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="60.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="61.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="36.109375" style="6" customWidth="1"/>
+    <col min="15" max="15" width="20.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18">
+    <row r="1" spans="1:14" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4931,7 +4931,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
@@ -4975,7 +4975,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
@@ -5019,7 +5019,7 @@
         <v>85.01</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
@@ -5063,7 +5063,7 @@
         <v>93.65</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>53</v>
       </c>
@@ -5107,7 +5107,7 @@
         <v>83.53</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>66</v>
       </c>
@@ -5151,7 +5151,7 @@
         <v>85.31</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>79</v>
       </c>
@@ -5195,7 +5195,7 @@
         <v>84.12</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>92</v>
       </c>
@@ -5239,7 +5239,7 @@
         <v>79.95</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>105</v>
       </c>
@@ -5283,7 +5283,7 @@
         <v>81.739999999999995</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>118</v>
       </c>
@@ -5327,7 +5327,7 @@
         <v>76.38</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>131</v>
       </c>
@@ -5371,7 +5371,7 @@
         <v>81.86</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>144</v>
       </c>
@@ -5415,7 +5415,7 @@
         <v>94.24</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>157</v>
       </c>
@@ -5459,7 +5459,7 @@
         <v>77.569999999999993</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>170</v>
       </c>
@@ -5503,7 +5503,7 @@
         <v>96.62</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>182</v>
       </c>
@@ -5547,7 +5547,7 @@
         <v>71.59</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>195</v>
       </c>
@@ -5591,7 +5591,7 @@
         <v>60.93</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>207</v>
       </c>
@@ -5635,7 +5635,7 @@
         <v>92.16</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>219</v>
       </c>
@@ -5679,7 +5679,7 @@
         <v>61.34</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>229</v>
       </c>
@@ -5723,7 +5723,7 @@
         <v>35.07</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>241</v>
       </c>
@@ -5767,7 +5767,7 @@
         <v>79.95</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>254</v>
       </c>
@@ -5811,7 +5811,7 @@
         <v>92.75</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>267</v>
       </c>
@@ -5855,7 +5855,7 @@
         <v>81.739999999999995</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>270</v>
       </c>
@@ -5899,7 +5899,7 @@
         <v>86.5</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>271</v>
       </c>
@@ -5943,83 +5943,83 @@
         <v>63.5</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="14.45">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="1:14" ht="14.45">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>286</v>
-      </c>
       <c r="D27" s="3" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="C28" t="s">
         <v>307</v>
       </c>
-      <c r="C28" t="s">
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="29" spans="1:14">
-      <c r="A29" s="3" t="s">
+      <c r="B29" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="C29" t="s">
         <v>310</v>
       </c>
-      <c r="C29" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" ht="14.45">
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="1:14" ht="14.45" customHeight="1">
+    <row r="32" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="C32" t="s">
         <v>294</v>
       </c>
-      <c r="C32" t="s">
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="8" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="8" t="s">
+      <c r="B33" s="27" t="s">
         <v>296</v>
-      </c>
-      <c r="B33" s="27" t="s">
-        <v>297</v>
       </c>
       <c r="C33" s="27"/>
       <c r="D33" s="27"/>
@@ -6042,30 +6042,30 @@
   <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B17" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B24" sqref="B24"/>
+      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="75.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="68.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="72.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="63.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="75.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="68.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="63.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="80" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="73.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="61.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="73.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="61.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="72" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="60.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="61.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="46.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="46.28515625" customWidth="1"/>
-    <col min="15" max="15" width="36.140625" style="6" customWidth="1"/>
-    <col min="16" max="16" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="60.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="61.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="46.33203125" customWidth="1"/>
+    <col min="15" max="15" width="36.109375" style="6" customWidth="1"/>
+    <col min="16" max="16" width="36.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="23" customFormat="1" ht="36">
+    <row r="1" spans="1:16" s="23" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -6106,16 +6106,16 @@
         <v>12</v>
       </c>
       <c r="N1" s="19" t="s">
+        <v>311</v>
+      </c>
+      <c r="O1" s="20" t="s">
         <v>312</v>
-      </c>
-      <c r="O1" s="20" t="s">
-        <v>313</v>
       </c>
       <c r="P1" s="22" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
@@ -6166,9 +6166,9 @@
         <v>0.93480000000000008</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B3" t="s">
         <v>28</v>
@@ -6217,7 +6217,7 @@
         <v>0.88700000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
@@ -6268,7 +6268,7 @@
         <v>0.90870000000000006</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>53</v>
       </c>
@@ -6319,7 +6319,7 @@
         <v>0.93910000000000005</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>66</v>
       </c>
@@ -6370,7 +6370,7 @@
         <v>0.87830000000000008</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>79</v>
       </c>
@@ -6421,7 +6421,7 @@
         <v>0.82169999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>92</v>
       </c>
@@ -6472,7 +6472,7 @@
         <v>0.88260000000000005</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>105</v>
       </c>
@@ -6523,7 +6523,7 @@
         <v>0.87609999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>118</v>
       </c>
@@ -6574,7 +6574,7 @@
         <v>0.84129999999999994</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>131</v>
       </c>
@@ -6625,7 +6625,7 @@
         <v>0.81299999999999994</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>144</v>
       </c>
@@ -6676,7 +6676,7 @@
         <v>0.92169999999999996</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>157</v>
       </c>
@@ -6727,7 +6727,7 @@
         <v>0.8478</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>170</v>
       </c>
@@ -6778,7 +6778,7 @@
         <v>0.92609999999999992</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>182</v>
       </c>
@@ -6829,7 +6829,7 @@
         <v>0.8609</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>195</v>
       </c>
@@ -6880,7 +6880,7 @@
         <v>0.8609</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>207</v>
       </c>
@@ -6931,7 +6931,7 @@
         <v>0.91300000000000003</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>219</v>
       </c>
@@ -6982,7 +6982,7 @@
         <v>0.91300000000000003</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>229</v>
       </c>
@@ -7033,7 +7033,7 @@
         <v>0.83909999999999996</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>241</v>
       </c>
@@ -7084,7 +7084,7 @@
         <v>0.80069999999999997</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>254</v>
       </c>
@@ -7135,7 +7135,7 @@
         <v>0.76390000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>267</v>
       </c>
@@ -7186,7 +7186,7 @@
         <v>0.86299999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>270</v>
       </c>
@@ -7237,7 +7237,7 @@
         <v>0.87830000000000008</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>271</v>
       </c>
@@ -7288,83 +7288,83 @@
         <v>0.91520000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>286</v>
-      </c>
       <c r="D27" s="3" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="C28" t="s">
         <v>316</v>
       </c>
-      <c r="C28" t="s">
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="29" spans="1:16">
-      <c r="A29" s="3" t="s">
+      <c r="B29" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="C29" t="s">
         <v>319</v>
       </c>
-      <c r="C29" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16">
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="1:16" ht="14.45" customHeight="1">
+    <row r="32" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="C32" t="s">
         <v>294</v>
       </c>
-      <c r="C32" t="s">
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="8" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="8" t="s">
+      <c r="B33" s="27" t="s">
         <v>296</v>
-      </c>
-      <c r="B33" s="27" t="s">
-        <v>297</v>
       </c>
       <c r="C33" s="27"/>
       <c r="D33" s="27"/>
@@ -7388,28 +7388,28 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N18" sqref="N18"/>
+      <selection pane="topRight" activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="75.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="68.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="72.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="63.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="75.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="68.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="63.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="80" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="73.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="61.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="73.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="61.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="72" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="60.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="61.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="46.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="36.140625" style="6" customWidth="1"/>
-    <col min="15" max="15" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="60.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="61.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="36.109375" style="6" customWidth="1"/>
+    <col min="15" max="15" width="20.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18">
+    <row r="1" spans="1:14" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -7450,10 +7450,10 @@
         <v>12</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
@@ -7497,7 +7497,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
@@ -7541,7 +7541,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
@@ -7585,7 +7585,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>53</v>
       </c>
@@ -7629,7 +7629,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>66</v>
       </c>
@@ -7673,7 +7673,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>79</v>
       </c>
@@ -7717,7 +7717,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>92</v>
       </c>
@@ -7761,7 +7761,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>105</v>
       </c>
@@ -7805,7 +7805,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>118</v>
       </c>
@@ -7849,7 +7849,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>131</v>
       </c>
@@ -7893,7 +7893,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>144</v>
       </c>
@@ -7937,7 +7937,7 @@
         <v>90.48</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>157</v>
       </c>
@@ -7981,7 +7981,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>170</v>
       </c>
@@ -8025,7 +8025,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>182</v>
       </c>
@@ -8069,7 +8069,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>195</v>
       </c>
@@ -8113,7 +8113,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>207</v>
       </c>
@@ -8157,7 +8157,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>219</v>
       </c>
@@ -8201,7 +8201,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>229</v>
       </c>
@@ -8245,7 +8245,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>241</v>
       </c>
@@ -8289,7 +8289,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>254</v>
       </c>
@@ -8333,7 +8333,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>267</v>
       </c>
@@ -8377,7 +8377,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>270</v>
       </c>
@@ -8421,7 +8421,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>271</v>
       </c>
@@ -8465,90 +8465,90 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="14.45">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="1:14" ht="14.45">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>286</v>
-      </c>
       <c r="D27" s="3" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="C28" t="s">
         <v>323</v>
       </c>
-      <c r="C28" t="s">
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="29" spans="1:14">
-      <c r="A29" s="3" t="s">
+      <c r="B29" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="C29" t="s">
         <v>326</v>
       </c>
-      <c r="C29" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" ht="14.45">
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="1:14" ht="14.45" customHeight="1">
+    <row r="32" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="C32" t="s">
         <v>294</v>
       </c>
-      <c r="C32" t="s">
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="8" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="8" t="s">
-        <v>296</v>
-      </c>
       <c r="B33" s="28" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C33" s="27"/>
       <c r="D33" s="27"/>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B34" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -8569,44 +8569,44 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="65" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>330</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>331</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>13</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="G1" s="18" t="s">
         <v>332</v>
       </c>
-      <c r="G1" s="18" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
@@ -8626,7 +8626,7 @@
       <c r="F2" s="14"/>
       <c r="G2" s="13"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
@@ -8650,7 +8650,7 @@
         <v>0.20730000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
@@ -8670,7 +8670,7 @@
       <c r="F4" s="14"/>
       <c r="G4" s="13"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>53</v>
       </c>
@@ -8690,7 +8690,7 @@
       <c r="F5" s="14"/>
       <c r="G5" s="13"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>66</v>
       </c>
@@ -8714,7 +8714,7 @@
         <v>0.31709999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>79</v>
       </c>
@@ -8738,7 +8738,7 @@
         <v>0.2195</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>92</v>
       </c>
@@ -8762,7 +8762,7 @@
         <v>0.25609999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>105</v>
       </c>
@@ -8782,7 +8782,7 @@
       <c r="F9" s="14"/>
       <c r="G9" s="13"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>118</v>
       </c>
@@ -8806,7 +8806,7 @@
         <v>0.29270000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>131</v>
       </c>
@@ -8830,7 +8830,7 @@
         <v>0.24390000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>144</v>
       </c>
@@ -8850,7 +8850,7 @@
       <c r="F12" s="14"/>
       <c r="G12" s="13"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>157</v>
       </c>
@@ -8874,7 +8874,7 @@
         <v>0.40239999999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>170</v>
       </c>
@@ -8894,7 +8894,7 @@
       <c r="F14" s="14"/>
       <c r="G14" s="13"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>182</v>
       </c>
@@ -8914,7 +8914,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="13"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>195</v>
       </c>
@@ -8938,7 +8938,7 @@
         <v>6.09</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>207</v>
       </c>
@@ -8958,7 +8958,7 @@
       <c r="F17" s="14"/>
       <c r="G17" s="13"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>219</v>
       </c>
@@ -8982,7 +8982,7 @@
         <v>0.27439999999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>229</v>
       </c>
@@ -9002,7 +9002,7 @@
       <c r="F19" s="14"/>
       <c r="G19" s="13"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>241</v>
       </c>
@@ -9022,7 +9022,7 @@
       <c r="F20" s="14"/>
       <c r="G20" s="13"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>254</v>
       </c>
@@ -9046,7 +9046,7 @@
         <v>0.32319999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>267</v>
       </c>
@@ -9066,7 +9066,7 @@
       <c r="F22" s="14"/>
       <c r="G22" s="13"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>270</v>
       </c>
@@ -9090,7 +9090,7 @@
         <v>0.189</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>271</v>
       </c>
@@ -9110,7 +9110,7 @@
       <c r="F24" s="14"/>
       <c r="G24" s="13"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="6">
@@ -9122,49 +9122,49 @@
         <v>0.29373913043478256</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>284</v>
+        <v>399</v>
       </c>
       <c r="B27" s="3"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="B28" s="3" t="s">
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="3" t="s">
+      <c r="B29" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B32" s="3"/>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B33" s="3"/>
     </row>
@@ -9180,41 +9180,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96AD7147-225E-44D0-A869-96828C996078}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="65" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="36.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="36">
+    <row r="1" spans="1:6" ht="36" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
+        <v>337</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>338</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="D1" s="18" t="s">
         <v>339</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>340</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>13</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
@@ -9232,7 +9232,7 @@
         <v>0.97900000000000009</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
@@ -9250,7 +9250,7 @@
         <v>0.74099999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
@@ -9268,7 +9268,7 @@
         <v>0.92999999999999994</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>53</v>
       </c>
@@ -9286,7 +9286,7 @@
         <v>0.90900000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>66</v>
       </c>
@@ -9304,7 +9304,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>79</v>
       </c>
@@ -9322,7 +9322,7 @@
         <v>0.83899999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>92</v>
       </c>
@@ -9340,7 +9340,7 @@
         <v>0.8600000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>105</v>
       </c>
@@ -9358,7 +9358,7 @@
         <v>0.68099999999999994</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>118</v>
       </c>
@@ -9376,7 +9376,7 @@
         <v>0.88100000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>131</v>
       </c>
@@ -9394,7 +9394,7 @@
         <v>0.71000000000000008</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>144</v>
       </c>
@@ -9412,7 +9412,7 @@
         <v>0.53900000000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>157</v>
       </c>
@@ -9430,7 +9430,7 @@
         <v>0.73099999999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>170</v>
       </c>
@@ -9448,7 +9448,7 @@
         <v>0.90900000000000003</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>182</v>
       </c>
@@ -9466,7 +9466,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>195</v>
       </c>
@@ -9484,7 +9484,7 @@
         <v>0.83899999999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>207</v>
       </c>
@@ -9502,10 +9502,10 @@
         <v>0.67900000000000005</v>
       </c>
       <c r="F17" s="26" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>219</v>
       </c>
@@ -9523,10 +9523,10 @@
         <v>0.441</v>
       </c>
       <c r="F18" s="26" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>229</v>
       </c>
@@ -9544,7 +9544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>241</v>
       </c>
@@ -9562,7 +9562,7 @@
         <v>0.66100000000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>254</v>
       </c>
@@ -9580,7 +9580,7 @@
         <v>0.90900000000000003</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>267</v>
       </c>
@@ -9598,7 +9598,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>270</v>
       </c>
@@ -9616,10 +9616,10 @@
         <v>0.63</v>
       </c>
       <c r="F23" s="26" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>271</v>
       </c>
@@ -9637,55 +9637,55 @@
         <v>0.88100000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="6"/>
       <c r="D25" s="12"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>284</v>
+        <v>399</v>
       </c>
       <c r="B27" s="3"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="B28" s="3" t="s">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="3" t="s">
+      <c r="B29" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B32" s="3"/>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B33" s="3"/>
     </row>
@@ -9702,42 +9702,42 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.7109375" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.140625" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.6640625" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.109375" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="B1" t="s">
         <v>347</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>348</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>349</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>350</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>351</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
         <v>352</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="10" t="s">
-        <v>353</v>
       </c>
       <c r="B2" s="6">
         <v>33.522727272727273</v>
@@ -9746,18 +9746,18 @@
         <v>100</v>
       </c>
       <c r="D2" s="9" t="s">
+        <v>353</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>354</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>355</v>
       </c>
       <c r="F2" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B3" s="6">
         <v>10.227272727272728</v>
@@ -9766,18 +9766,18 @@
         <v>72.02</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F3" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B4" s="6">
         <v>9.0909090909090917</v>
@@ -9786,18 +9786,18 @@
         <v>89.29</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F4" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B5" s="6">
         <v>13.636363636363635</v>
@@ -9806,16 +9806,16 @@
         <v>69.05</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F5" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>66</v>
       </c>
@@ -9826,18 +9826,18 @@
         <v>72.62</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F6" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B7" s="6">
         <v>6.8181818181818175</v>
@@ -9846,18 +9846,18 @@
         <v>70.239999999999995</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F7" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B8" s="6">
         <v>30.681818181818183</v>
@@ -9866,18 +9866,18 @@
         <v>61.9</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F8" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B9" s="6">
         <v>19.318181818181817</v>
@@ -9886,18 +9886,18 @@
         <v>65.48</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F9" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B10" s="6">
         <v>0</v>
@@ -9906,38 +9906,38 @@
         <v>54.76</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F10" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B11" s="6">
         <v>10.795454545454545</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F11" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B12" s="6">
         <v>17.045454545454543</v>
@@ -9946,18 +9946,18 @@
         <v>90.48</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F12" s="11">
         <v>0.97960000000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B13" s="6">
         <v>12.5</v>
@@ -9966,18 +9966,18 @@
         <v>57.14</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F13" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B14" s="6">
         <v>21.59090909090909</v>
@@ -9986,18 +9986,18 @@
         <v>95.24</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F14" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B15" s="6">
         <v>44.31818181818182</v>
@@ -10006,18 +10006,18 @@
         <v>62.5</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F15" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B16" s="6">
         <v>15.909090909090908</v>
@@ -10026,18 +10026,18 @@
         <v>44.05</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F16" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B17" s="6">
         <v>25</v>
@@ -10046,18 +10046,18 @@
         <v>86.31</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F17" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B18" s="6">
         <v>13.636363636363635</v>
@@ -10066,18 +10066,18 @@
         <v>43.45</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F18" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B19" s="6">
         <v>10.227272727272728</v>
@@ -10086,18 +10086,18 @@
         <v>26.79</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F19" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B20" s="6">
         <v>6.8181818181818175</v>
@@ -10106,18 +10106,18 @@
         <v>61.9</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F20" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B21" s="6">
         <v>15.909090909090908</v>
@@ -10126,18 +10126,18 @@
         <v>87.5</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F21" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B22" s="6">
         <v>17.045454545454543</v>
@@ -10146,18 +10146,18 @@
         <v>65.48</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F22" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B23" s="6">
         <v>19.318181818181817</v>
@@ -10166,18 +10166,18 @@
         <v>75</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F23" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B24" s="6">
         <v>22.727272727272727</v>
@@ -10186,19 +10186,19 @@
         <v>48.21</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E24" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="F24" s="11" t="s">
         <v>398</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>399</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{176341A8-A8A0-42CB-B3F9-C4E249DECF8A}"/>
-    <hyperlink ref="E3:E24" r:id="rId2" xr:uid="{A8EBCD7E-0A33-4356-ACD6-85C43BAD297C}"/>
+    <hyperlink ref="E3:E24" r:id="rId2" display="https://sharing.clickup.com/90181072599/b/h/6-901808512021-2/959c2149d211a26" xr:uid="{A8EBCD7E-0A33-4356-ACD6-85C43BAD297C}"/>
     <hyperlink ref="D2" r:id="rId3" xr:uid="{67C0B007-D6A0-4A20-BABD-48BCB8BEC7C4}"/>
     <hyperlink ref="D3:D24" r:id="rId4" display="https://github.com/CodelineAtyab/Brain360/pulls?q=is%3Apr+is%3Aclosed" xr:uid="{1B7EE5F9-42D0-4CF0-ABF0-1CC65A465CE5}"/>
   </hyperlinks>
@@ -10207,6 +10207,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="5524ecfe-089c-425a-a4be-7743da73ddfc" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7112d4b0-5493-499c-a8a1-c4cefa8f8360">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CC4386AB3068CD42B8F0F14A3B25C6E6" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1b0865c603b059e198cdfbdcd5fd1e24">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7112d4b0-5493-499c-a8a1-c4cefa8f8360" xmlns:ns3="5524ecfe-089c-425a-a4be-7743da73ddfc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b01538475ea0a03af6b38dbffea6db4f" ns2:_="" ns3:_="">
     <xsd:import namespace="7112d4b0-5493-499c-a8a1-c4cefa8f8360"/>
@@ -10441,34 +10461,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="5524ecfe-089c-425a-a4be-7743da73ddfc" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7112d4b0-5493-499c-a8a1-c4cefa8f8360">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1003B133-145C-44E0-99DB-E235C0D8382C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40E2C60B-4EB2-4AA1-9F0B-5016388626E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF181BE1-4349-4356-BB20-D498CEDB0838}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF181BE1-4349-4356-BB20-D498CEDB0838}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5524ecfe-089c-425a-a4be-7743da73ddfc"/>
+    <ds:schemaRef ds:uri="7112d4b0-5493-499c-a8a1-c4cefa8f8360"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40E2C60B-4EB2-4AA1-9F0B-5016388626E9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1003B133-145C-44E0-99DB-E235C0D8382C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="7112d4b0-5493-499c-a8a1-c4cefa8f8360"/>
+    <ds:schemaRef ds:uri="5524ecfe-089c-425a-a4be-7743da73ddfc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>